<commit_message>
Updated solution for Tutorial 6
</commit_message>
<xml_diff>
--- a/tut06/output/2001CB02.xlsx
+++ b/tut06/output/2001CB02.xlsx
@@ -496,13 +496,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>28/07/2022</t>
+          <t>28-07-2022</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -511,7 +511,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -520,16 +520,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01/08/2022</t>
+          <t>01-08-2022</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -538,22 +538,22 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>04/08/2022</t>
+          <t>04-08-2022</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -562,22 +562,22 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>08/08/2022</t>
+          <t>08-08-2022</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -586,13 +586,13 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>11/08/2022</t>
+          <t>11-08-2022</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -616,7 +616,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>15/08/2022</t>
+          <t>15-08-2022</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -640,7 +640,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18/08/2022</t>
+          <t>18-08-2022</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -664,7 +664,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>22/08/2022</t>
+          <t>22-08-2022</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -688,16 +688,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>25/08/2022</t>
+          <t>25-08-2022</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -706,13 +706,13 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>29/08/2022</t>
+          <t>29-08-2022</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -736,7 +736,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>01/09/2022</t>
+          <t>01-09-2022</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -760,16 +760,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05/09/2022</t>
+          <t>05-09-2022</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -778,19 +778,19 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>08/09/2022</t>
+          <t>08-09-2022</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
@@ -808,13 +808,13 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>12/09/2022</t>
+          <t>12-09-2022</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -823,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
@@ -832,7 +832,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>15/09/2022</t>
+          <t>15-09-2022</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -856,7 +856,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19/09/2022</t>
+          <t>19-09-2022</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -880,7 +880,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>22-09-2022</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -904,16 +904,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>26-09-2022</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -922,19 +922,19 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>29/09/2022</t>
+          <t>29-09-2022</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>1</v>

</xml_diff>